<commit_message>
muchas cosas a ya...
</commit_message>
<xml_diff>
--- a/DIMECRES_C_retrovisors.xlsx
+++ b/DIMECRES_C_retrovisors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5d53d53a2166798a/Documentos/GitHub/DIMECRES_C_retrovisors/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="327" documentId="8_{5367DCFB-67D5-4F12-89D8-6F4F7588B090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A65C46DD-D7AF-4C74-979C-FCE38B44785F}"/>
+  <xr:revisionPtr revIDLastSave="406" documentId="8_{5367DCFB-67D5-4F12-89D8-6F4F7588B090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5771B5B9-8A36-4C29-A609-58305B7A9CA0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7DC49289-096D-4701-9CE4-62A406282F74}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="266">
   <si>
     <t>TOTAL COMPONENTS:   (€/placa)</t>
   </si>
@@ -196,9 +196,6 @@
     <t>PREU FINAL</t>
   </si>
   <si>
-    <t>TOTAL PCB:  (€/placa)</t>
-  </si>
-  <si>
     <t>Stencils</t>
   </si>
   <si>
@@ -815,6 +812,36 @@
   </si>
   <si>
     <t>C5542957</t>
+  </si>
+  <si>
+    <t>TOTAL PCB</t>
+  </si>
+  <si>
+    <t>x20000</t>
+  </si>
+  <si>
+    <t>Capacitats</t>
+  </si>
+  <si>
+    <t>Resistències</t>
+  </si>
+  <si>
+    <t>Inductància</t>
+  </si>
+  <si>
+    <t>Altres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x </t>
+  </si>
+  <si>
+    <t>x1000</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -976,7 +1003,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1192,8 +1219,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="39">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -1643,6 +1676,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1689,7 +1737,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1734,18 +1782,12 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1770,12 +1812,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1783,6 +1819,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1794,19 +1833,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="39" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2234,10 +2286,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7C1BA9-9B92-4979-86A8-F02E41774D04}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1:U1048576"/>
+    <sheetView tabSelected="1" topLeftCell="E23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R48" sqref="R48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2260,143 +2313,143 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
         <v>64</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>65</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>66</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>67</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>69</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" s="64" t="s">
+      <c r="B2" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="D2" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" s="64" t="s">
-        <v>74</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
         <v>75</v>
       </c>
-      <c r="G2" s="64" t="s">
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="B3" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
         <v>73</v>
-      </c>
-      <c r="D3" s="64" t="s">
-        <v>74</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="64" t="s">
+      <c r="F3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A4" s="64" t="s">
+      <c r="B4" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
         <v>81</v>
-      </c>
-      <c r="C4" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="64" t="s">
-        <v>82</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
-      <c r="F4" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="64" t="s">
-        <v>83</v>
+      <c r="F4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>82</v>
       </c>
       <c r="J4" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="64" t="s">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="C5" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="64" t="s">
-        <v>82</v>
+      <c r="C5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" t="s">
+        <v>81</v>
       </c>
       <c r="E5">
         <v>7</v>
       </c>
-      <c r="F5" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="64" t="s">
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="6" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="64" t="s">
+      <c r="B6" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
         <v>88</v>
-      </c>
-      <c r="C6" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="64" t="s">
-        <v>89</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="64" t="s">
-        <v>90</v>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" t="s">
+        <v>89</v>
       </c>
       <c r="J6" s="16" t="s">
         <v>47</v>
@@ -2415,26 +2468,26 @@
       </c>
     </row>
     <row r="7" spans="1:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="64" t="s">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="64" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="64" t="s">
-        <v>89</v>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>88</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="64" t="s">
-        <v>93</v>
+      <c r="F7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G7" t="s">
+        <v>92</v>
       </c>
       <c r="J7" s="13" t="s">
         <v>42</v>
@@ -2445,26 +2498,26 @@
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="64" t="s">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="64" t="s">
-        <v>95</v>
-      </c>
-      <c r="C8" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>82</v>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
-      <c r="F8" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" s="64" t="s">
-        <v>96</v>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="s">
+        <v>95</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>41</v>
@@ -2482,33 +2535,33 @@
         <v>7.27</v>
       </c>
       <c r="O8" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P8" s="28" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="64" t="s">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" t="s">
         <v>97</v>
       </c>
-      <c r="B9" s="64" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="64" t="s">
-        <v>89</v>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="64" t="s">
-        <v>99</v>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="s">
+        <v>98</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>39</v>
@@ -2526,33 +2579,33 @@
         <v>6.6509999999999998</v>
       </c>
       <c r="O9" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P9" s="29" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="64" t="s">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
         <v>100</v>
       </c>
-      <c r="B10" s="64" t="s">
-        <v>101</v>
-      </c>
-      <c r="C10" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="64" t="s">
-        <v>89</v>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" t="s">
+        <v>88</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
-      <c r="F10" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="64" t="s">
-        <v>102</v>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" t="s">
+        <v>101</v>
       </c>
       <c r="J10" s="5" t="s">
         <v>37</v>
@@ -2570,33 +2623,33 @@
         <v>1.026</v>
       </c>
       <c r="O10" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P10" s="29" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="64" t="s">
-        <v>103</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>85</v>
-      </c>
-      <c r="C11" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="64" t="s">
-        <v>89</v>
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" t="s">
+        <v>88</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G11" s="64" t="s">
-        <v>104</v>
+      <c r="F11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" t="s">
+        <v>103</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>35</v>
@@ -2614,33 +2667,33 @@
         <v>1.48</v>
       </c>
       <c r="O11" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P11" s="29" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="64" t="s">
+      <c r="A12" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" t="s">
         <v>105</v>
-      </c>
-      <c r="B12" s="64" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="64" t="s">
-        <v>106</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" s="64" t="s">
-        <v>107</v>
+      <c r="F12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" t="s">
+        <v>106</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>33</v>
@@ -2658,33 +2711,33 @@
         <v>2.5449999999999999</v>
       </c>
       <c r="O12" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P12" s="29" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="64" t="s">
+      <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="64" t="s">
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="s">
         <v>109</v>
-      </c>
-      <c r="C13" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="64" t="s">
-        <v>110</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" s="64" t="s">
-        <v>111</v>
+      <c r="F13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" t="s">
+        <v>110</v>
       </c>
       <c r="J13" s="5" t="s">
         <v>31</v>
@@ -2702,33 +2755,33 @@
         <v>1.17</v>
       </c>
       <c r="O13" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P13" s="29" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="64" t="s">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
         <v>112</v>
       </c>
-      <c r="B14" s="64" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="64" t="s">
+      <c r="D14" t="s">
         <v>113</v>
-      </c>
-      <c r="D14" s="64" t="s">
-        <v>114</v>
       </c>
       <c r="E14">
         <v>3</v>
       </c>
-      <c r="F14" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" s="64" t="s">
-        <v>115</v>
+      <c r="F14" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" t="s">
+        <v>114</v>
       </c>
       <c r="J14" s="5" t="s">
         <v>29</v>
@@ -2746,33 +2799,33 @@
         <v>3.06</v>
       </c>
       <c r="O14" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P14" s="29" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="64" t="s">
+      <c r="A15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B15" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="64" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="64" t="s">
-        <v>110</v>
+      <c r="C15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" t="s">
+        <v>109</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="64" t="s">
-        <v>118</v>
+      <c r="F15" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" t="s">
+        <v>117</v>
       </c>
       <c r="J15" s="5" t="s">
         <v>27</v>
@@ -2790,7 +2843,7 @@
         <v>3.71</v>
       </c>
       <c r="O15" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P15" s="29" t="s">
         <v>26</v>
@@ -2798,26 +2851,26 @@
       <c r="AB15" s="35"/>
     </row>
     <row r="16" spans="1:28" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="64" t="s">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
         <v>119</v>
       </c>
-      <c r="B16" s="64" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="64" t="s">
+      <c r="D16" t="s">
         <v>120</v>
-      </c>
-      <c r="D16" s="64" t="s">
-        <v>121</v>
       </c>
       <c r="E16">
         <v>8</v>
       </c>
-      <c r="F16" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="64" t="s">
-        <v>75</v>
+      <c r="F16" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" t="s">
+        <v>74</v>
       </c>
       <c r="J16" s="5" t="s">
         <v>25</v>
@@ -2835,33 +2888,33 @@
         <v>7.1499999999999994E-2</v>
       </c>
       <c r="O16" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P16" s="29" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="64" t="s">
+      <c r="A17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B17" t="s">
         <v>122</v>
       </c>
-      <c r="B17" s="64" t="s">
+      <c r="C17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" t="s">
         <v>123</v>
-      </c>
-      <c r="C17" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="64" t="s">
-        <v>124</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
-      <c r="F17" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="64" t="s">
-        <v>125</v>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" t="s">
+        <v>124</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>23</v>
@@ -2879,33 +2932,33 @@
         <v>3.1E-2</v>
       </c>
       <c r="O17" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P17" s="29" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="64" t="s">
+      <c r="A18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" t="s">
         <v>126</v>
       </c>
-      <c r="B18" s="64" t="s">
+      <c r="C18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
         <v>127</v>
-      </c>
-      <c r="C18" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D18" s="64" t="s">
-        <v>128</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="64" t="s">
-        <v>129</v>
+      <c r="F18" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s">
+        <v>128</v>
       </c>
       <c r="J18" s="5" t="s">
         <v>21</v>
@@ -2923,33 +2976,33 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="O18" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P18" s="29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="64" t="s">
+      <c r="A19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" t="s">
         <v>130</v>
       </c>
-      <c r="B19" s="64" t="s">
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" t="s">
         <v>131</v>
-      </c>
-      <c r="C19" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="64" t="s">
-        <v>132</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="64" t="s">
-        <v>133</v>
+      <c r="F19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" t="s">
+        <v>132</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>19</v>
@@ -2967,33 +3020,33 @@
         <v>0.754</v>
       </c>
       <c r="O19" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P19" s="29" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="64" t="s">
+      <c r="A20" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="64" t="s">
-        <v>135</v>
-      </c>
-      <c r="C20" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" s="64" t="s">
-        <v>132</v>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>131</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="64" t="s">
-        <v>133</v>
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+      <c r="G20" t="s">
+        <v>132</v>
       </c>
       <c r="J20" s="5" t="s">
         <v>17</v>
@@ -3011,33 +3064,33 @@
         <v>4.65E-2</v>
       </c>
       <c r="O20" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P20" s="29" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="64" t="s">
+      <c r="A21" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="64" t="s">
-        <v>137</v>
-      </c>
-      <c r="C21" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="64" t="s">
-        <v>132</v>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" t="s">
+        <v>131</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="64" t="s">
-        <v>133</v>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="G21" t="s">
+        <v>132</v>
       </c>
       <c r="J21" s="5" t="s">
         <v>15</v>
@@ -3055,33 +3108,33 @@
         <v>0.09</v>
       </c>
       <c r="O21" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P21" s="29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="64" t="s">
+      <c r="A22" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" t="s">
         <v>138</v>
       </c>
-      <c r="B22" s="64" t="s">
-        <v>139</v>
-      </c>
-      <c r="C22" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D22" s="64" t="s">
-        <v>132</v>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" s="64" t="s">
-        <v>133</v>
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" t="s">
+        <v>132</v>
       </c>
       <c r="J22" s="5" t="s">
         <v>13</v>
@@ -3099,33 +3152,33 @@
         <v>3.6900000000000002E-2</v>
       </c>
       <c r="O22" s="32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P22" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="64" t="s">
+      <c r="A23" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" t="s">
         <v>140</v>
       </c>
-      <c r="B23" s="64" t="s">
-        <v>141</v>
-      </c>
-      <c r="C23" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D23" s="64" t="s">
-        <v>132</v>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" t="s">
+        <v>131</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" s="64" t="s">
-        <v>133</v>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" t="s">
+        <v>132</v>
       </c>
       <c r="J23" s="5" t="s">
         <v>11</v>
@@ -3143,33 +3196,33 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="O23" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P23" s="29" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="64" t="s">
+      <c r="A24" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" t="s">
         <v>142</v>
       </c>
-      <c r="B24" s="64" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D24" s="64" t="s">
-        <v>132</v>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24" t="s">
+        <v>131</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="64" t="s">
-        <v>133</v>
+      <c r="F24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G24" t="s">
+        <v>132</v>
       </c>
       <c r="J24" s="8" t="s">
         <v>9</v>
@@ -3187,33 +3240,33 @@
         <v>0.93899999999999995</v>
       </c>
       <c r="O24" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P24" s="29" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="64" t="s">
+      <c r="A25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" t="s">
         <v>144</v>
       </c>
-      <c r="B25" s="64" t="s">
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" t="s">
         <v>145</v>
-      </c>
-      <c r="C25" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="64" t="s">
-        <v>146</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" s="64" t="s">
-        <v>129</v>
+      <c r="F25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" t="s">
+        <v>128</v>
       </c>
       <c r="J25" s="8" t="s">
         <v>7</v>
@@ -3231,33 +3284,33 @@
         <v>0.105</v>
       </c>
       <c r="O25" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P25" s="29" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="64" t="s">
+      <c r="A26" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" t="s">
         <v>147</v>
       </c>
-      <c r="B26" s="64" t="s">
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" t="s">
         <v>148</v>
-      </c>
-      <c r="C26" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="64" t="s">
-        <v>149</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" s="64" t="s">
-        <v>150</v>
+      <c r="F26" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" t="s">
+        <v>149</v>
       </c>
       <c r="J26" s="5" t="s">
         <v>5</v>
@@ -3275,33 +3328,33 @@
         <v>0.13700000000000001</v>
       </c>
       <c r="O26" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P26" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="64" t="s">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
         <v>151</v>
       </c>
-      <c r="B27" s="64" t="s">
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D27" t="s">
         <v>152</v>
-      </c>
-      <c r="C27" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" s="64" t="s">
-        <v>153</v>
       </c>
       <c r="E27">
         <v>3</v>
       </c>
-      <c r="F27" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="64" t="s">
-        <v>154</v>
+      <c r="F27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" t="s">
+        <v>153</v>
       </c>
       <c r="J27" s="5" t="s">
         <v>3</v>
@@ -3319,33 +3372,33 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="O27" s="34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P27" s="29" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="64" t="s">
+      <c r="A28" t="s">
+        <v>154</v>
+      </c>
+      <c r="B28" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="64" t="s">
+      <c r="C28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" t="s">
         <v>156</v>
-      </c>
-      <c r="C28" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" s="64" t="s">
-        <v>157</v>
       </c>
       <c r="E28">
         <v>5</v>
       </c>
-      <c r="F28" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G28" s="64" t="s">
-        <v>158</v>
+      <c r="F28" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" t="s">
+        <v>157</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>1</v>
@@ -3353,7 +3406,7 @@
       <c r="K28" s="2">
         <v>5.3330000000000002</v>
       </c>
-      <c r="L28" s="58">
+      <c r="L28" s="36">
         <v>4.76</v>
       </c>
       <c r="M28" s="1">
@@ -3362,34 +3415,34 @@
       <c r="N28" s="27">
         <v>4.5309999999999997</v>
       </c>
-      <c r="O28" s="59" t="s">
-        <v>62</v>
+      <c r="O28" s="37" t="s">
+        <v>61</v>
       </c>
       <c r="P28" s="30" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="64" t="s">
+      <c r="A29" t="s">
+        <v>158</v>
+      </c>
+      <c r="B29" t="s">
         <v>159</v>
       </c>
-      <c r="B29" s="64" t="s">
-        <v>160</v>
-      </c>
-      <c r="C29" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="64" t="s">
-        <v>157</v>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="s">
+        <v>156</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G29" s="64" t="s">
-        <v>161</v>
+      <c r="F29" t="s">
+        <v>74</v>
+      </c>
+      <c r="G29" t="s">
+        <v>160</v>
       </c>
       <c r="J29" s="13" t="s">
         <v>0</v>
@@ -3406,473 +3459,537 @@
         <f t="shared" si="0"/>
         <v>52.059899999999992</v>
       </c>
-      <c r="N29" s="63">
+      <c r="N29" s="41">
         <f t="shared" si="0"/>
         <v>50.963899999999995</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="64" t="s">
+      <c r="A30" t="s">
+        <v>161</v>
+      </c>
+      <c r="B30" t="s">
         <v>162</v>
       </c>
-      <c r="B30" s="64" t="s">
-        <v>163</v>
-      </c>
-      <c r="C30" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D30" s="64" t="s">
-        <v>157</v>
+      <c r="C30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="s">
+        <v>156</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="F30" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="64" t="s">
-        <v>164</v>
-      </c>
-      <c r="J30" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="K30" s="62">
+      <c r="F30" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" t="s">
+        <v>163</v>
+      </c>
+      <c r="J30" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="K30" s="40">
         <f>K29*10</f>
         <v>653.5</v>
       </c>
-      <c r="L30" s="62">
+      <c r="L30" s="40">
         <f>L29*50</f>
         <v>3044.0999999999995</v>
       </c>
-      <c r="M30" s="62">
+      <c r="M30" s="40">
         <f>M29*1000</f>
         <v>52059.899999999994</v>
       </c>
-      <c r="N30" s="61">
+      <c r="N30" s="39">
         <f>N29*20000</f>
         <v>1019277.9999999999</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="64" t="s">
+      <c r="A31" t="s">
+        <v>164</v>
+      </c>
+      <c r="B31" t="s">
         <v>165</v>
       </c>
-      <c r="B31" s="64" t="s">
-        <v>166</v>
-      </c>
-      <c r="C31" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="64" t="s">
-        <v>157</v>
+      <c r="C31" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>156</v>
       </c>
       <c r="E31">
         <v>2</v>
       </c>
-      <c r="F31" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G31" s="64" t="s">
+      <c r="F31" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="64" t="s">
+      <c r="B32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" s="64" t="s">
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
         <v>169</v>
-      </c>
-      <c r="C32" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D32" s="64" t="s">
-        <v>170</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G32" s="64" t="s">
+      <c r="F32" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="64" t="s">
+      <c r="B33" t="s">
         <v>172</v>
       </c>
-      <c r="B33" s="64" t="s">
-        <v>173</v>
-      </c>
-      <c r="C33" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="64" t="s">
-        <v>157</v>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="s">
+        <v>156</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="F33" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G33" s="64" t="s">
+      <c r="F33" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="64" t="s">
+      <c r="B34" t="s">
         <v>175</v>
       </c>
-      <c r="B34" s="64" t="s">
-        <v>176</v>
-      </c>
-      <c r="C34" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="64" t="s">
-        <v>157</v>
+      <c r="C34" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" t="s">
+        <v>156</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="F34" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G34" s="64" t="s">
+      <c r="F34" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A35" s="64" t="s">
+      <c r="B35" t="s">
         <v>178</v>
       </c>
-      <c r="B35" s="64" t="s">
-        <v>179</v>
-      </c>
-      <c r="C35" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="64" t="s">
-        <v>170</v>
+      <c r="C35" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" t="s">
+        <v>169</v>
       </c>
       <c r="E35">
         <v>4</v>
       </c>
-      <c r="F35" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G35" s="64" t="s">
+      <c r="F35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G35" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="64" t="s">
+      <c r="B36" t="s">
         <v>181</v>
       </c>
-      <c r="B36" s="64" t="s">
-        <v>182</v>
-      </c>
-      <c r="C36" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="64" t="s">
-        <v>157</v>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" t="s">
+        <v>156</v>
       </c>
       <c r="E36">
         <v>4</v>
       </c>
-      <c r="F36" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G36" s="64" t="s">
+      <c r="F36" t="s">
+        <v>74</v>
+      </c>
+      <c r="G36" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A37" s="64" t="s">
+      <c r="B37" t="s">
         <v>184</v>
       </c>
-      <c r="B37" s="64" t="s">
-        <v>185</v>
-      </c>
-      <c r="C37" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D37" s="64" t="s">
-        <v>170</v>
+      <c r="C37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D37" t="s">
+        <v>169</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G37" s="64" t="s">
+      <c r="F37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G37" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A38" s="64" t="s">
+      <c r="B38" t="s">
         <v>187</v>
       </c>
-      <c r="B38" s="64" t="s">
-        <v>188</v>
-      </c>
-      <c r="C38" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="64" t="s">
-        <v>170</v>
+      <c r="C38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" t="s">
+        <v>169</v>
       </c>
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" s="64" t="s">
+      <c r="F38" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A39" s="64" t="s">
+      <c r="B39" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="64" t="s">
-        <v>191</v>
-      </c>
-      <c r="C39" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D39" s="64" t="s">
-        <v>170</v>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>169</v>
       </c>
       <c r="E39">
         <v>2</v>
       </c>
-      <c r="F39" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G39" s="64" t="s">
+      <c r="F39" t="s">
+        <v>74</v>
+      </c>
+      <c r="G39" t="s">
+        <v>191</v>
+      </c>
+      <c r="J39" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
         <v>192</v>
       </c>
-      <c r="J39" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="64" t="s">
+      <c r="B40" t="s">
         <v>193</v>
       </c>
-      <c r="B40" s="64" t="s">
-        <v>194</v>
-      </c>
-      <c r="C40" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="64" t="s">
-        <v>170</v>
+      <c r="C40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" t="s">
+        <v>169</v>
       </c>
       <c r="E40">
         <v>1</v>
       </c>
-      <c r="F40" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G40" s="64" t="s">
+      <c r="F40" t="s">
+        <v>74</v>
+      </c>
+      <c r="G40" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="41" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="64" t="s">
+      <c r="B41" t="s">
         <v>196</v>
       </c>
-      <c r="B41" s="64" t="s">
+      <c r="C41" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" t="s">
         <v>197</v>
-      </c>
-      <c r="C41" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="64" t="s">
-        <v>198</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G41" s="64" t="s">
+      <c r="F41" t="s">
+        <v>74</v>
+      </c>
+      <c r="G41" t="s">
+        <v>198</v>
+      </c>
+      <c r="K41" s="42" t="s">
+        <v>53</v>
+      </c>
+      <c r="L41" s="43"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="44"/>
+      <c r="O41" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="P41" s="43"/>
+      <c r="Q41" s="43"/>
+      <c r="R41" s="44"/>
+      <c r="T41" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="U41" s="66" t="s">
+        <v>258</v>
+      </c>
+      <c r="V41" s="66" t="s">
+        <v>259</v>
+      </c>
+      <c r="W41" s="66" t="s">
+        <v>260</v>
+      </c>
+      <c r="X41" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y41" s="66" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
         <v>199</v>
       </c>
-      <c r="K41" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="L41" s="41"/>
-      <c r="M41" s="41"/>
-      <c r="N41" s="42"/>
-      <c r="O41" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="P41" s="41"/>
-      <c r="Q41" s="41"/>
-      <c r="R41" s="42"/>
-    </row>
-    <row r="42" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="64" t="s">
+      <c r="B42" t="s">
         <v>200</v>
       </c>
-      <c r="B42" s="64" t="s">
+      <c r="C42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" t="s">
         <v>201</v>
-      </c>
-      <c r="C42" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D42" s="64" t="s">
-        <v>202</v>
       </c>
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="64" t="s">
-        <v>203</v>
+      <c r="F42" t="s">
+        <v>74</v>
+      </c>
+      <c r="G42" t="s">
+        <v>202</v>
       </c>
       <c r="J42" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="K42" s="40" t="s">
+      <c r="K42" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="L42" s="42"/>
-      <c r="M42" s="40" t="s">
+      <c r="L42" s="44"/>
+      <c r="M42" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="N42" s="42"/>
-      <c r="O42" s="40" t="s">
+      <c r="N42" s="44"/>
+      <c r="O42" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="P42" s="42"/>
-      <c r="Q42" s="40" t="s">
+      <c r="P42" s="44"/>
+      <c r="Q42" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="R42" s="42"/>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A43" s="64" t="s">
+      <c r="R42" s="44"/>
+      <c r="T42" s="64" t="s">
+        <v>263</v>
+      </c>
+      <c r="U42" s="64" t="s">
+        <v>265</v>
+      </c>
+      <c r="V42" s="64" t="s">
+        <v>265</v>
+      </c>
+      <c r="W42" s="64" t="s">
+        <v>265</v>
+      </c>
+      <c r="X42" s="64">
+        <f>1000*(M16+7*M25+M19+M9+M13+M15+M27+2*M28+6*M24+2*M11+M18+M8+M26)</f>
+        <v>43876.5</v>
+      </c>
+      <c r="Y42" s="64">
+        <f>SUM(U42:X42)</f>
+        <v>43876.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>203</v>
+      </c>
+      <c r="B43" t="s">
         <v>204</v>
       </c>
-      <c r="B43" s="64" t="s">
-        <v>205</v>
-      </c>
-      <c r="C43" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="64" t="s">
-        <v>202</v>
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" t="s">
+        <v>201</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="F43" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G43" s="64" t="s">
-        <v>203</v>
+      <c r="F43" t="s">
+        <v>74</v>
+      </c>
+      <c r="G43" t="s">
+        <v>202</v>
       </c>
       <c r="J43" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="K43" s="38">
+        <v>55</v>
+      </c>
+      <c r="K43" s="59">
         <f>K29*10</f>
         <v>653.5</v>
       </c>
-      <c r="L43" s="39"/>
+      <c r="L43" s="53"/>
       <c r="M43" s="52">
         <f>L29*50</f>
         <v>3044.0999999999995</v>
       </c>
-      <c r="N43" s="39"/>
+      <c r="N43" s="53"/>
       <c r="O43" s="52">
-        <f>M29*1000</f>
-        <v>52059.899999999994</v>
-      </c>
-      <c r="P43" s="39"/>
-      <c r="Q43" s="54">
-        <f>N29*20000</f>
-        <v>1019277.9999999999</v>
-      </c>
-      <c r="R43" s="55"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A44" s="64" t="s">
+        <f>Y42</f>
+        <v>43876.5</v>
+      </c>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="55">
+        <f>Y43</f>
+        <v>928537.99999999988</v>
+      </c>
+      <c r="R43" s="56"/>
+      <c r="T43" s="65" t="s">
+        <v>257</v>
+      </c>
+      <c r="U43" s="65">
+        <f>2842+156+3648+864+432</f>
+        <v>7942</v>
+      </c>
+      <c r="V43" s="65">
+        <f>38+14</f>
+        <v>52</v>
+      </c>
+      <c r="W43" s="65">
+        <v>364</v>
+      </c>
+      <c r="X43" s="65">
+        <f>20000*(N16+3*N20+8*N21+3*N17+N12+2*N11+7*N25+N19+N14+N9+N8+N10+2*N28+6*N24+N18+N26+N27)</f>
+        <v>920179.99999999988</v>
+      </c>
+      <c r="Y43" s="65">
+        <f>SUM(U43:X43)</f>
+        <v>928537.99999999988</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>205</v>
+      </c>
+      <c r="B44" t="s">
         <v>206</v>
       </c>
-      <c r="B44" s="64" t="s">
-        <v>207</v>
-      </c>
-      <c r="C44" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D44" s="64" t="s">
-        <v>202</v>
+      <c r="C44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" t="s">
+        <v>201</v>
       </c>
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="F44" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G44" s="64" t="s">
-        <v>203</v>
+      <c r="F44" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" t="s">
+        <v>202</v>
       </c>
       <c r="J44" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="K44" s="53" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="K44" s="54" t="s">
+        <v>56</v>
       </c>
       <c r="L44" s="51"/>
       <c r="M44" s="50">
         <v>64.7</v>
       </c>
       <c r="N44" s="51"/>
-      <c r="O44" s="50"/>
+      <c r="O44" s="50">
+        <v>502.8</v>
+      </c>
       <c r="P44" s="51"/>
-      <c r="Q44" s="56"/>
-      <c r="R44" s="57"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A45" s="64" t="s">
+      <c r="Q44" s="62">
+        <v>7749.8</v>
+      </c>
+      <c r="R44" s="63"/>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>207</v>
+      </c>
+      <c r="B45" t="s">
         <v>208</v>
       </c>
-      <c r="B45" s="64" t="s">
-        <v>209</v>
-      </c>
-      <c r="C45" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D45" s="64" t="s">
-        <v>202</v>
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
+        <v>201</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
-      <c r="F45" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G45" s="64" t="s">
-        <v>203</v>
+      <c r="F45" t="s">
+        <v>74</v>
+      </c>
+      <c r="G45" t="s">
+        <v>202</v>
       </c>
       <c r="J45" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="K45" s="53">
+        <v>50</v>
+      </c>
+      <c r="K45" s="54">
         <v>7</v>
       </c>
       <c r="L45" s="51"/>
@@ -3881,390 +3998,417 @@
       </c>
       <c r="N45" s="51"/>
       <c r="O45" s="50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P45" s="51"/>
-      <c r="Q45" s="56" t="s">
-        <v>58</v>
-      </c>
-      <c r="R45" s="57"/>
-    </row>
-    <row r="46" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="64" t="s">
+      <c r="Q45" s="62" t="s">
+        <v>262</v>
+      </c>
+      <c r="R45" s="63"/>
+    </row>
+    <row r="46" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>209</v>
+      </c>
+      <c r="B46" t="s">
         <v>210</v>
       </c>
-      <c r="B46" s="64" t="s">
-        <v>211</v>
-      </c>
-      <c r="C46" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D46" s="64" t="s">
-        <v>202</v>
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+      <c r="D46" t="s">
+        <v>201</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
-      <c r="F46" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G46" s="64" t="s">
-        <v>203</v>
+      <c r="F46" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46" t="s">
+        <v>202</v>
       </c>
       <c r="J46" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="K46" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="L46" s="44"/>
-      <c r="M46" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="N46" s="44"/>
-      <c r="O46" s="46"/>
-      <c r="P46" s="44"/>
-      <c r="Q46" s="46"/>
-      <c r="R46" s="47"/>
-    </row>
-    <row r="47" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="64" t="s">
+      <c r="K46" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="L46" s="46"/>
+      <c r="M46" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="N46" s="46"/>
+      <c r="O46" s="48">
+        <v>3515.34</v>
+      </c>
+      <c r="P46" s="46"/>
+      <c r="Q46" s="48">
+        <v>9097.65</v>
+      </c>
+      <c r="R46" s="49"/>
+    </row>
+    <row r="47" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B47" t="s">
         <v>212</v>
       </c>
-      <c r="B47" s="64" t="s">
-        <v>213</v>
-      </c>
-      <c r="C47" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="64" t="s">
-        <v>202</v>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" t="s">
+        <v>201</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
-      <c r="F47" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G47" s="64" t="s">
-        <v>203</v>
+      <c r="F47" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" t="s">
+        <v>202</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="K47" s="48">
-        <f>SUM(K43:L45)</f>
+        <v>256</v>
+      </c>
+      <c r="K47" s="60">
+        <f>SUM(K43:L46)</f>
         <v>660.5</v>
       </c>
-      <c r="L47" s="49"/>
-      <c r="M47" s="48">
-        <f>SUM(M43:N45)</f>
+      <c r="L47" s="61"/>
+      <c r="M47" s="60">
+        <f>SUM(M43:N46)</f>
         <v>3115.7999999999993</v>
       </c>
-      <c r="N47" s="49"/>
-      <c r="O47" s="48">
-        <f>SUM(O43:P45)</f>
-        <v>52059.899999999994</v>
-      </c>
-      <c r="P47" s="49"/>
-      <c r="Q47" s="48">
-        <f>SUM(Q43:R45)</f>
-        <v>1019277.9999999999</v>
-      </c>
-      <c r="R47" s="49"/>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="64" t="s">
+      <c r="N47" s="61"/>
+      <c r="O47" s="60">
+        <f>SUM(O43:P46)</f>
+        <v>47894.64</v>
+      </c>
+      <c r="P47" s="61"/>
+      <c r="Q47" s="60">
+        <f>SUM(Q43:R46)</f>
+        <v>945385.45</v>
+      </c>
+      <c r="R47" s="61"/>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>213</v>
+      </c>
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="C48" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" t="s">
         <v>214</v>
-      </c>
-      <c r="B48" s="64" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="64" t="s">
-        <v>215</v>
       </c>
       <c r="E48">
         <v>2</v>
       </c>
-      <c r="F48" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G48" s="64" t="s">
-        <v>75</v>
+      <c r="F48" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="64" t="s">
+      <c r="A49" t="s">
+        <v>215</v>
+      </c>
+      <c r="B49" t="s">
         <v>216</v>
       </c>
-      <c r="B49" s="64" t="s">
-        <v>217</v>
-      </c>
-      <c r="C49" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D49" s="64" t="s">
-        <v>202</v>
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" t="s">
+        <v>201</v>
       </c>
       <c r="E49">
         <v>1</v>
       </c>
-      <c r="F49" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G49" s="64" t="s">
-        <v>203</v>
+      <c r="F49" t="s">
+        <v>74</v>
+      </c>
+      <c r="G49" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="64" t="s">
+      <c r="A50" t="s">
+        <v>217</v>
+      </c>
+      <c r="B50" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" t="s">
         <v>218</v>
-      </c>
-      <c r="B50" s="64" t="s">
-        <v>20</v>
-      </c>
-      <c r="C50" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="D50" s="64" t="s">
-        <v>219</v>
       </c>
       <c r="E50">
         <v>1</v>
       </c>
-      <c r="F50" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G50" s="64" t="s">
-        <v>220</v>
+      <c r="F50" t="s">
+        <v>74</v>
+      </c>
+      <c r="G50" t="s">
+        <v>219</v>
       </c>
       <c r="J50" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="K50" s="36"/>
-      <c r="L50" s="37"/>
-      <c r="M50" s="36">
+      <c r="K50" s="57">
+        <f>K47/10</f>
+        <v>66.05</v>
+      </c>
+      <c r="L50" s="58"/>
+      <c r="M50" s="57">
         <f>M47/50</f>
         <v>62.315999999999988</v>
       </c>
-      <c r="N50" s="37"/>
-      <c r="O50" s="36"/>
-      <c r="P50" s="37"/>
-      <c r="Q50" s="36"/>
-      <c r="R50" s="37"/>
+      <c r="N50" s="58"/>
+      <c r="O50" s="57">
+        <f>O47/1000</f>
+        <v>47.894640000000003</v>
+      </c>
+      <c r="P50" s="58"/>
+      <c r="Q50" s="57">
+        <f>Q47/20000</f>
+        <v>47.2692725</v>
+      </c>
+      <c r="R50" s="58"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A51" s="64" t="s">
+      <c r="A51" t="s">
+        <v>220</v>
+      </c>
+      <c r="B51" t="s">
+        <v>18</v>
+      </c>
+      <c r="C51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" t="s">
         <v>221</v>
-      </c>
-      <c r="B51" s="64" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="64" t="s">
-        <v>222</v>
       </c>
       <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G51" s="64" t="s">
+      <c r="F51" t="s">
+        <v>74</v>
+      </c>
+      <c r="G51" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A52" s="64" t="s">
+      <c r="B52" t="s">
         <v>224</v>
       </c>
-      <c r="B52" s="64" t="s">
+      <c r="C52" t="s">
         <v>225</v>
       </c>
-      <c r="C52" s="64" t="s">
+      <c r="D52" t="s">
         <v>226</v>
-      </c>
-      <c r="D52" s="64" t="s">
-        <v>227</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G52" s="64" t="s">
+      <c r="F52" t="s">
+        <v>74</v>
+      </c>
+      <c r="G52" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A53" s="64" t="s">
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" t="s">
         <v>229</v>
       </c>
-      <c r="B53" s="64" t="s">
-        <v>38</v>
-      </c>
-      <c r="C53" s="64" t="s">
+      <c r="D53" t="s">
         <v>230</v>
-      </c>
-      <c r="D53" s="64" t="s">
-        <v>231</v>
       </c>
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G53" s="64" t="s">
+      <c r="F53" t="s">
+        <v>74</v>
+      </c>
+      <c r="G53" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A54" s="64" t="s">
+      <c r="B54" t="s">
         <v>233</v>
       </c>
-      <c r="B54" s="64" t="s">
+      <c r="C54" t="s">
         <v>234</v>
       </c>
-      <c r="C54" s="64" t="s">
+      <c r="D54" t="s">
         <v>235</v>
-      </c>
-      <c r="D54" s="64" t="s">
-        <v>236</v>
       </c>
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G54" s="64" t="s">
+      <c r="F54" t="s">
+        <v>74</v>
+      </c>
+      <c r="G54" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A55" s="64" t="s">
+      <c r="B55" t="s">
+        <v>30</v>
+      </c>
+      <c r="C55" t="s">
         <v>238</v>
       </c>
-      <c r="B55" s="64" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" s="64" t="s">
-        <v>239</v>
-      </c>
-      <c r="D55" s="64" t="s">
-        <v>236</v>
+      <c r="D55" t="s">
+        <v>235</v>
       </c>
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G55" s="64" t="s">
+      <c r="F55" t="s">
+        <v>74</v>
+      </c>
+      <c r="G55" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A56" s="64" t="s">
+      <c r="B56" t="s">
         <v>241</v>
       </c>
-      <c r="B56" s="64" t="s">
+      <c r="C56" t="s">
         <v>242</v>
       </c>
-      <c r="C56" s="64" t="s">
+      <c r="D56" t="s">
         <v>243</v>
-      </c>
-      <c r="D56" s="64" t="s">
-        <v>244</v>
       </c>
       <c r="E56">
         <v>1</v>
       </c>
-      <c r="F56" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G56" s="64" t="s">
+      <c r="F56" t="s">
+        <v>74</v>
+      </c>
+      <c r="G56" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A57" s="64" t="s">
+      <c r="B57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" t="s">
         <v>246</v>
-      </c>
-      <c r="B57" s="64" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="D57" s="64" t="s">
-        <v>247</v>
       </c>
       <c r="E57">
         <v>1</v>
       </c>
-      <c r="F57" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G57" s="64" t="s">
-        <v>75</v>
+      <c r="F57" t="s">
+        <v>74</v>
+      </c>
+      <c r="G57" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A58" s="64" t="s">
+      <c r="A58" t="s">
+        <v>247</v>
+      </c>
+      <c r="B58" t="s">
         <v>248</v>
       </c>
-      <c r="B58" s="64" t="s">
+      <c r="C58" t="s">
         <v>249</v>
       </c>
-      <c r="C58" s="64" t="s">
+      <c r="D58" t="s">
         <v>250</v>
-      </c>
-      <c r="D58" s="64" t="s">
-        <v>251</v>
       </c>
       <c r="E58">
         <v>1</v>
       </c>
-      <c r="F58" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G58" s="64" t="s">
+      <c r="F58" t="s">
+        <v>74</v>
+      </c>
+      <c r="G58" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A59" s="64" t="s">
+      <c r="B59" t="s">
         <v>253</v>
       </c>
-      <c r="B59" s="64" t="s">
+      <c r="C59" t="s">
+        <v>72</v>
+      </c>
+      <c r="D59" t="s">
         <v>254</v>
-      </c>
-      <c r="C59" s="64" t="s">
-        <v>73</v>
-      </c>
-      <c r="D59" s="64" t="s">
-        <v>255</v>
       </c>
       <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59" s="64" t="s">
-        <v>75</v>
-      </c>
-      <c r="G59" s="64" t="s">
-        <v>256</v>
+      <c r="F59" t="s">
+        <v>74</v>
+      </c>
+      <c r="G59" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="O50:P50"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="K43:L43"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="O47:P47"/>
+    <mergeCell ref="K47:L47"/>
+    <mergeCell ref="M43:N43"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="M45:N45"/>
     <mergeCell ref="O41:R41"/>
     <mergeCell ref="K41:N41"/>
     <mergeCell ref="K46:L46"/>
@@ -4281,20 +4425,6 @@
     <mergeCell ref="M42:N42"/>
     <mergeCell ref="O42:P42"/>
     <mergeCell ref="Q42:R42"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="M50:N50"/>
-    <mergeCell ref="O50:P50"/>
-    <mergeCell ref="Q50:R50"/>
-    <mergeCell ref="K43:L43"/>
-    <mergeCell ref="M47:N47"/>
-    <mergeCell ref="O47:P47"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="M43:N43"/>
-    <mergeCell ref="Q44:R44"/>
-    <mergeCell ref="Q45:R45"/>
-    <mergeCell ref="Q47:R47"/>
-    <mergeCell ref="M44:N44"/>
-    <mergeCell ref="M45:N45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="P8" r:id="rId1" xr:uid="{ADF289B5-44B3-4B8A-8E2B-50174AE55933}"/>

</xml_diff>